<commit_message>
fix(place): add sample queries
actually the sample do not query by place

see #15
</commit_message>
<xml_diff>
--- a/notes/Ranking_Stabikat.xlsx
+++ b/notes/Ranking_Stabikat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Wo wollen wir hin"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="242">
   <si>
     <t xml:space="preserve">Nr. </t>
   </si>
@@ -54,6 +54,9 @@
 absteigend chronologisch als erstes Relevanzkriterium, ergänzend als 2. Autor mit den meisten Publikationen im Index</t>
   </si>
   <si>
+    <t>x</t>
+  </si>
+  <si>
     <t>soziale frauenschule berlin</t>
   </si>
   <si>
@@ -265,9 +268,6 @@
   </si>
   <si>
     <t>Matomo: Title</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>history berlin / geschichte berlin</t>
@@ -1929,7 +1929,7 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2058,7 +2058,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>107</v>
@@ -2079,7 +2079,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>111</v>
@@ -2091,7 +2091,7 @@
         <v>105</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>113</v>
@@ -2102,7 +2102,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>114</v>
@@ -2133,7 +2133,7 @@
         <v>120</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>121</v>
@@ -2165,7 +2165,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>127</v>
@@ -2177,7 +2177,7 @@
         <v>129</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G13" s="4"/>
     </row>
@@ -2186,7 +2186,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>130</v>
@@ -2207,7 +2207,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>134</v>
@@ -2219,7 +2219,7 @@
         <v>116</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G15" s="4"/>
     </row>
@@ -2228,7 +2228,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>136</v>
@@ -2238,7 +2238,7 @@
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>138</v>
@@ -2249,7 +2249,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>139</v>
@@ -2258,10 +2258,10 @@
         <v>140</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G17" s="4"/>
     </row>
@@ -2278,7 +2278,7 @@
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G18" s="4"/>
     </row>
@@ -2287,7 +2287,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>143</v>
@@ -2299,7 +2299,7 @@
         <v>116</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G19" s="4"/>
     </row>
@@ -2318,7 +2318,7 @@
         <v>147</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G20" s="4"/>
     </row>
@@ -2335,7 +2335,7 @@
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G21" s="4"/>
     </row>
@@ -2344,7 +2344,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>150</v>
@@ -2354,7 +2354,7 @@
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G22" s="4"/>
     </row>
@@ -2363,7 +2363,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>152</v>
@@ -2458,7 +2458,7 @@
   </sheetPr>
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2529,19 +2529,21 @@
       <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C5" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="33">
@@ -2550,17 +2552,17 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="33">
@@ -2569,19 +2571,19 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="60.75">
@@ -2590,19 +2592,19 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
@@ -2611,16 +2613,16 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -2629,19 +2631,19 @@
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -2651,16 +2653,16 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="G11" s="4"/>
     </row>
@@ -2670,19 +2672,19 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
@@ -2690,10 +2692,10 @@
       <c r="B13" s="2"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="4"/>
@@ -2704,19 +2706,19 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="F14" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="33">
@@ -2725,13 +2727,13 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="4"/>
@@ -2742,16 +2744,16 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G16" s="4"/>
     </row>
@@ -2761,16 +2763,16 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="G17" s="4"/>
     </row>
@@ -2780,16 +2782,16 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G18" s="4"/>
     </row>
@@ -2799,14 +2801,14 @@
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G19" s="4"/>
     </row>
@@ -2816,16 +2818,16 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G20" s="4"/>
     </row>
@@ -2835,16 +2837,16 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G21" s="4"/>
     </row>
@@ -2854,16 +2856,16 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G22" s="4"/>
     </row>
@@ -2873,16 +2875,16 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G23" s="4"/>
     </row>
@@ -2892,16 +2894,16 @@
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G24" s="4"/>
     </row>
@@ -2911,16 +2913,16 @@
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G25" s="4"/>
     </row>
@@ -2929,19 +2931,19 @@
         <v>21</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C26" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="F26" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G26" s="4"/>
     </row>
@@ -2950,7 +2952,7 @@
         <v>22</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>78</v>
@@ -2968,7 +2970,9 @@
       <c r="A28" s="6">
         <v>23</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C28" s="4" t="s">
         <v>81</v>
       </c>
@@ -2983,7 +2987,9 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5" customFormat="1" s="13">
       <c r="A29" s="15"/>
-      <c r="B29" s="4"/>
+      <c r="B29" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="C29" s="4" t="s">
         <v>84</v>
       </c>
@@ -2992,14 +2998,14 @@
         <v>85</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G29" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5" customFormat="1" s="13">
       <c r="A30" s="15"/>
       <c r="B30" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
ci: add new specs
</commit_message>
<xml_diff>
--- a/notes/Ranking_Stabikat.xlsx
+++ b/notes/Ranking_Stabikat.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="242">
   <si>
     <t xml:space="preserve">Nr. </t>
   </si>
@@ -2324,7 +2324,9 @@
       <c r="A21" s="5">
         <v>18</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C21" s="2" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
fix(chronolgy): finish chrono import
see #35 #11 #40 #39
</commit_message>
<xml_diff>
--- a/notes/Ranking_Stabikat.xlsx
+++ b/notes/Ranking_Stabikat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Wo wollen wir hin"/>
@@ -1917,7 +1917,7 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="G23" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="4"/>
@@ -2401,7 +2401,7 @@
         <v>155</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="4"/>
@@ -2410,7 +2410,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="4"/>
@@ -2419,7 +2419,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="4"/>
@@ -2458,7 +2458,7 @@
   </sheetPr>
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>